<commit_message>
Database Structure update spreadsheet
Just something I quickly did during my free's. Doesn't modify the code
at all, just concept for the new database design. :3
</commit_message>
<xml_diff>
--- a/Project/Database Structure.xlsx
+++ b/Project/Database Structure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WindowsDocs\Documents\GitHub\Classics-2014\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\CMS\Classics-2014\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Events</t>
   </si>
@@ -41,63 +41,101 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Options</t>
-  </si>
-  <si>
     <t>Competitors</t>
   </si>
   <si>
     <t>UID</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
     <t>Nationality</t>
   </si>
   <si>
-    <t>Event Specific</t>
-  </si>
-  <si>
-    <t>Accuracy Landings</t>
-  </si>
-  <si>
-    <t>LandingID</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
-    <t>Wind Data</t>
-  </si>
-  <si>
-    <t>int, unique</t>
-  </si>
-  <si>
-    <t>int unique</t>
-  </si>
-  <si>
-    <t>serialised ruleset</t>
-  </si>
-  <si>
-    <t>Accuracy, etc.</t>
-  </si>
-  <si>
-    <t>serialised</t>
-  </si>
-  <si>
-    <t>Event EVENTID</t>
-  </si>
-  <si>
-    <t>LandingID/ScoreID</t>
+    <t>Things that need to be stored:</t>
+  </si>
+  <si>
+    <t>Landings</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>Key:</t>
+  </si>
+  <si>
+    <t>Rejumpable</t>
+  </si>
+  <si>
+    <t>Could be serialised, useful in raw form</t>
+  </si>
+  <si>
+    <t>Event Teams</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>FakeCompetitorEnumerator</t>
+  </si>
+  <si>
+    <t>Age? Competing Level?</t>
+  </si>
+  <si>
+    <t>Required, visible in table</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>String (int?)</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>string/int</t>
+  </si>
+  <si>
+    <t>Could/Should competitors be serialised?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,13 +158,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,11 +181,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,102 +468,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>